<commit_message>
Supplemental transect draw post power analysis
</commit_message>
<xml_diff>
--- a/Oyster/transect/data/supp_trans_2019_final.xlsx
+++ b/Oyster/transect/data/supp_trans_2019_final.xlsx
@@ -62,12 +62,6 @@
     <t>LCI28-1</t>
   </si>
   <si>
-    <t>LTI</t>
-  </si>
-  <si>
-    <t>LTI-2</t>
-  </si>
-  <si>
     <t>LCI29</t>
   </si>
   <si>
@@ -92,12 +86,6 @@
     <t>NNI6-1</t>
   </si>
   <si>
-    <t>LTI10</t>
-  </si>
-  <si>
-    <t>LTI10-1</t>
-  </si>
-  <si>
     <t>LCI30</t>
   </si>
   <si>
@@ -183,6 +171,18 @@
   </si>
   <si>
     <t>SUPPLEMENTAL TRANSECT CHECKLIST</t>
+  </si>
+  <si>
+    <t>LTI3</t>
+  </si>
+  <si>
+    <t>LTI3-2</t>
+  </si>
+  <si>
+    <t>LTI12</t>
+  </si>
+  <si>
+    <t>LTI12-1</t>
   </si>
 </sst>
 </file>
@@ -190,7 +190,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -239,7 +239,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -522,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +535,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -558,10 +558,10 @@
         <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>2</v>
@@ -575,7 +575,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1">
         <v>3</v>
@@ -590,7 +590,7 @@
         <v>21.663311879999998</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H3" s="1">
         <v>297876.4375</v>
@@ -599,7 +599,7 @@
         <v>3239054.5639999998</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -607,7 +607,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C4" s="1">
         <v>3</v>
@@ -622,7 +622,7 @@
         <v>21.663311879999998</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H4" s="1">
         <v>297876.4375</v>
@@ -631,7 +631,7 @@
         <v>3239032.9010000001</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -639,7 +639,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C5" s="1">
         <v>2</v>
@@ -654,7 +654,7 @@
         <v>16.884199280000001</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H5" s="1">
         <v>298858.21629999997</v>
@@ -663,7 +663,7 @@
         <v>3235735.733</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -671,7 +671,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
@@ -686,7 +686,7 @@
         <v>16.884199280000001</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H6" s="1">
         <v>298841.3321</v>
@@ -695,7 +695,7 @@
         <v>3235735.733</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -703,7 +703,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
@@ -718,7 +718,7 @@
         <v>21.516840370000001</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H7" s="1">
         <v>298891.20169999998</v>
@@ -727,7 +727,7 @@
         <v>3235561.733</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -735,7 +735,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
@@ -750,7 +750,7 @@
         <v>21.516840370000001</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H8" s="1">
         <v>298869.68479999999</v>
@@ -759,7 +759,7 @@
         <v>3235561.733</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -767,7 +767,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
@@ -782,7 +782,7 @@
         <v>23.733760799999999</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H9" s="1">
         <v>298601.90519999998</v>
@@ -791,7 +791,7 @@
         <v>3235561.733</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -799,7 +799,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C10" s="1">
         <v>2</v>
@@ -814,7 +814,7 @@
         <v>23.733760799999999</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H10" s="1">
         <v>298578.1715</v>
@@ -823,7 +823,7 @@
         <v>3235561.733</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -846,7 +846,7 @@
         <v>14.017176660000001</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H11" s="1">
         <v>299022.4375</v>
@@ -878,7 +878,7 @@
         <v>14.017176660000001</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H12" s="1">
         <v>299022.4375</v>
@@ -895,7 +895,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C13" s="1">
         <v>1</v>
@@ -910,7 +910,7 @@
         <v>42.221868469999997</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H13" s="1">
         <v>298888.4375</v>
@@ -919,7 +919,7 @@
         <v>3235426.4640000002</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -927,7 +927,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C14" s="1">
         <v>2</v>
@@ -942,7 +942,7 @@
         <v>31.56563744</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H14" s="1">
         <v>298890.60220000002</v>
@@ -951,7 +951,7 @@
         <v>3235403.733</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -959,7 +959,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C15" s="1">
         <v>1</v>
@@ -974,7 +974,7 @@
         <v>42.221868469999997</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H15" s="1">
         <v>298888.4375</v>
@@ -983,7 +983,7 @@
         <v>3235384.2420000001</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -991,7 +991,7 @@
         <v>2</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C16" s="1">
         <v>2</v>
@@ -1006,7 +1006,7 @@
         <v>31.56563744</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H16" s="1">
         <v>298859.03659999999</v>
@@ -1015,7 +1015,7 @@
         <v>3235403.733</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1023,7 +1023,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C17" s="1">
         <v>3</v>
@@ -1038,7 +1038,7 @@
         <v>31.54447579</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H17" s="1">
         <v>298766.4375</v>
@@ -1047,7 +1047,7 @@
         <v>3235640.9649999999</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1055,7 +1055,7 @@
         <v>2</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C18" s="1">
         <v>3</v>
@@ -1070,7 +1070,7 @@
         <v>31.54447579</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H18" s="1">
         <v>298766.4375</v>
@@ -1079,7 +1079,7 @@
         <v>3235609.42</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1087,7 +1087,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C19" s="1">
         <v>1</v>
@@ -1102,7 +1102,7 @@
         <v>38.163140249999998</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H19" s="1">
         <v>299226.4375</v>
@@ -1111,7 +1111,7 @@
         <v>3235562.1030000001</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1119,7 +1119,7 @@
         <v>2</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C20" s="1">
         <v>1</v>
@@ -1134,7 +1134,7 @@
         <v>38.163140249999998</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H20" s="1">
         <v>299226.4375</v>
@@ -1143,7 +1143,7 @@
         <v>3235523.94</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1151,7 +1151,7 @@
         <v>2</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C21" s="1">
         <v>1</v>
@@ -1166,7 +1166,7 @@
         <v>34.10873325</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H21" s="1">
         <v>298074.4375</v>
@@ -1175,7 +1175,7 @@
         <v>3235364.412</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1183,7 +1183,7 @@
         <v>2</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C22" s="1">
         <v>1</v>
@@ -1198,7 +1198,7 @@
         <v>34.10873325</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H22" s="1">
         <v>298074.4375</v>
@@ -1207,7 +1207,7 @@
         <v>3235330.304</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1215,7 +1215,7 @@
         <v>2</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C23" s="1">
         <v>1</v>
@@ -1230,7 +1230,7 @@
         <v>34.299833370000002</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H23" s="1">
         <v>298730.4375</v>
@@ -1239,7 +1239,7 @@
         <v>3235981.18</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1247,7 +1247,7 @@
         <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C24" s="1">
         <v>1</v>
@@ -1262,7 +1262,7 @@
         <v>34.299833370000002</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H24" s="1">
         <v>298730.4375</v>
@@ -1271,7 +1271,7 @@
         <v>3235946.88</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1279,7 +1279,7 @@
         <v>2</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C25" s="1">
         <v>1</v>
@@ -1294,7 +1294,7 @@
         <v>10.76442701</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H25" s="1">
         <v>298315.946</v>
@@ -1303,7 +1303,7 @@
         <v>3236221.733</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1311,7 +1311,7 @@
         <v>2</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C26" s="1">
         <v>1</v>
@@ -1326,7 +1326,7 @@
         <v>10.76442701</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H26" s="1">
         <v>298305.18160000001</v>
@@ -1335,7 +1335,7 @@
         <v>3236221.733</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1343,7 +1343,7 @@
         <v>2</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C27" s="1">
         <v>2</v>
@@ -1358,7 +1358,7 @@
         <v>28.534128039999999</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H27" s="1">
         <v>297761.89689999999</v>
@@ -1367,7 +1367,7 @@
         <v>3234653.733</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -1375,7 +1375,7 @@
         <v>2</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C28" s="1">
         <v>2</v>
@@ -1390,7 +1390,7 @@
         <v>28.534128039999999</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H28" s="1">
         <v>297733.3628</v>
@@ -1399,7 +1399,7 @@
         <v>3234653.733</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -1407,7 +1407,7 @@
         <v>2</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C29" s="1">
         <v>1</v>
@@ -1422,7 +1422,7 @@
         <v>52.548068319999999</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H29" s="1">
         <v>297903.32909999997</v>
@@ -1431,7 +1431,7 @@
         <v>3234631.733</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -1439,7 +1439,7 @@
         <v>2</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C30" s="1">
         <v>1</v>
@@ -1454,7 +1454,7 @@
         <v>52.548068319999999</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H30" s="1">
         <v>297850.78100000002</v>
@@ -1463,7 +1463,7 @@
         <v>3234631.733</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -1471,7 +1471,7 @@
         <v>2</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C31" s="1">
         <v>2</v>
@@ -1486,7 +1486,7 @@
         <v>12.6140928</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H31" s="1">
         <v>298633.82199999999</v>
@@ -1495,7 +1495,7 @@
         <v>3236495.733</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -1503,7 +1503,7 @@
         <v>2</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C32" s="1">
         <v>2</v>
@@ -1518,7 +1518,7 @@
         <v>12.6140928</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H32" s="1">
         <v>298621.20789999998</v>
@@ -1527,7 +1527,7 @@
         <v>3236495.733</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -1535,7 +1535,7 @@
         <v>2</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="C33" s="1">
         <v>2</v>
@@ -1550,7 +1550,7 @@
         <v>18.25205369</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H33" s="1">
         <v>298352.38579999999</v>
@@ -1559,7 +1559,7 @@
         <v>3238419.733</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -1567,7 +1567,7 @@
         <v>2</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="C34" s="1">
         <v>2</v>
@@ -1582,7 +1582,7 @@
         <v>18.25205369</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H34" s="1">
         <v>298334.13370000001</v>
@@ -1591,7 +1591,7 @@
         <v>3238419.733</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -1599,7 +1599,7 @@
         <v>2</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="C35" s="1">
         <v>1</v>
@@ -1614,7 +1614,7 @@
         <v>17.778081270000001</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H35" s="1">
         <v>298450.31079999998</v>
@@ -1623,7 +1623,7 @@
         <v>3238083.733</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -1631,7 +1631,7 @@
         <v>2</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="C36" s="1">
         <v>1</v>
@@ -1646,7 +1646,7 @@
         <v>17.778081270000001</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H36" s="1">
         <v>298432.53269999998</v>
@@ -1655,7 +1655,7 @@
         <v>3238083.733</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -1663,7 +1663,7 @@
         <v>2</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C37" s="1">
         <v>1</v>
@@ -1678,7 +1678,7 @@
         <v>12.471459060000001</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H37" s="1">
         <v>298484.4375</v>
@@ -1687,7 +1687,7 @@
         <v>3237644.8849999998</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -1695,7 +1695,7 @@
         <v>2</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C38" s="1">
         <v>2</v>
@@ -1710,7 +1710,7 @@
         <v>12.043912819999999</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H38" s="1">
         <v>298528.4375</v>
@@ -1719,7 +1719,7 @@
         <v>3237707.7259999998</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -1727,7 +1727,7 @@
         <v>2</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C39" s="1">
         <v>1</v>
@@ -1742,7 +1742,7 @@
         <v>12.471459060000001</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H39" s="1">
         <v>298484.4375</v>
@@ -1751,7 +1751,7 @@
         <v>3237632.4130000002</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -1759,7 +1759,7 @@
         <v>2</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C40" s="1">
         <v>2</v>
@@ -1774,7 +1774,7 @@
         <v>12.043912819999999</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H40" s="1">
         <v>298528.4375</v>
@@ -1783,7 +1783,7 @@
         <v>3237695.682</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -1791,7 +1791,7 @@
         <v>2</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C41" s="1">
         <v>1</v>
@@ -1806,7 +1806,7 @@
         <v>25.589159949999999</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H41" s="1">
         <v>298532.94199999998</v>
@@ -1815,7 +1815,7 @@
         <v>3237737.733</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -1823,7 +1823,7 @@
         <v>2</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C42" s="1">
         <v>1</v>
@@ -1838,7 +1838,7 @@
         <v>25.589159949999999</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H42" s="1">
         <v>298507.3529</v>
@@ -1847,7 +1847,7 @@
         <v>3237737.733</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>